<commit_message>
added SMUD prices to 2005
</commit_message>
<xml_diff>
--- a/Fig6_ResRateTimeSeries/SummerBaselineTieredRate.xlsx
+++ b/Fig6_ResRateTimeSeries/SummerBaselineTieredRate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayan/Developer/CCAResearch/ConsolidatedPrimerData/CA_electricity_primer/Fig6_ResRateTimeSeries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646FF83D-19E5-284F-B062-D28F6DB640EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F00B370-658E-B24E-AC90-15A45CAAE0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12760" windowHeight="17500" xr2:uid="{2ED96552-DAFC-C646-85A2-7A03F356D192}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" xr2:uid="{2ED96552-DAFC-C646-85A2-7A03F356D192}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="23">
   <si>
     <t>Utility</t>
   </si>
@@ -74,18 +74,6 @@
     <t>CPA-SC</t>
   </si>
   <si>
-    <t>https://apps.openei.org/USURDB/rate/view/539f7506ec4f024411ed0f81#1__Basic_Information</t>
-  </si>
-  <si>
-    <t>https://apps.openei.org/USURDB/rate/view/565533075457a36b7b947b74#3__Energy</t>
-  </si>
-  <si>
-    <t>https://apps.openei.org/USURDB/rate/view/587e3b795457a33352316ce6#3__Energy</t>
-  </si>
-  <si>
-    <t>https://apps.openei.org/USURDB/rate/view/5a38163f5457a3af54d2dd7e</t>
-  </si>
-  <si>
     <t>https://rates.ladwp.com/UserFiles/Rate%20Summaries/Simplified%20Electric%20Rates/Simplified%20Electric%20Rates%202019-2021%20Oct%202021.pdf</t>
   </si>
   <si>
@@ -95,29 +83,35 @@
     <t>https://rates.ladwp.com/UserFiles/Rate%20Summaries/Simplified%20Electric%20Rates/Simplified%20Electric%20Rates%202019-2024%20Jan%202024.pdf</t>
   </si>
   <si>
-    <t>https://apps.openei.org/USURDB/rate/view/62c852e709e7863b6f399106#1__Basic_Information</t>
-  </si>
-  <si>
     <t>https://www.smud.org/en/Rate-Information/Residential-rates/Fixed-Rate</t>
   </si>
   <si>
-    <t>https://apps.openei.org/USURDB/rate/view/5dbc7d375457a3f842dc72bb</t>
-  </si>
-  <si>
-    <t>https://apps.openei.org/USURDB/rate/view/5c48887c5457a3641242792d</t>
-  </si>
-  <si>
-    <t>https://apps.openei.org/USURDB/rate/view/5a54f0555457a3674e423a7c</t>
-  </si>
-  <si>
-    <t>https://apps.openei.org/USURDB/rate/view/587e927e5457a31645316ce6#3__Energy</t>
+    <t>https://www.smud.org/-/media/Documents/Corporate/About-Us/Company-Information/Reports-and-Documents/GM-Reports/2015-GM-Rate-Report-Vol-1.ashx</t>
+  </si>
+  <si>
+    <t>https://www.smud.org/-/media/Documents/Corporate/About-Us/Company-Information/Reports-and-Documents/GM-Reports/2017-GM-Rate-Report-Vol-2.ashx</t>
+  </si>
+  <si>
+    <t>https://www.smud.org/-/media/Documents/Corporate/About-Us/Company-Information/Reports-and-Documents/Rates-Resolution-18-09-09.ashx</t>
+  </si>
+  <si>
+    <t>https://www.smud.org/-/media/Documents/Corporate/About-Us/Company-Information/Reports-and-Documents/2014-2021/2021/SMUD-General-Resolution-No-21-09-06.ashx</t>
+  </si>
+  <si>
+    <t>https://www.smud.org/-/media/Documents/Rate-Information/Rate-Archive/Resolution-No-190601.ashx</t>
+  </si>
+  <si>
+    <t>Email from SMUD</t>
+  </si>
+  <si>
+    <t>PDFs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -150,6 +144,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -188,6 +188,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C765326C-66C9-9B4E-AA2F-2EFB2434479E}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +535,7 @@
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -558,8 +559,11 @@
       <c r="C2">
         <v>0.1143</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -569,8 +573,11 @@
       <c r="C3">
         <v>0.1143</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -580,8 +587,11 @@
       <c r="C4">
         <v>0.1143</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -591,8 +601,11 @@
       <c r="C5" s="3">
         <v>0.11559999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -602,8 +615,11 @@
       <c r="C6" s="3">
         <v>0.11536</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -613,8 +629,11 @@
       <c r="C7" s="3">
         <v>0.11877</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -624,8 +643,11 @@
       <c r="C8" s="3">
         <v>0.12232999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -635,8 +657,11 @@
       <c r="C9" s="3">
         <v>0.12845000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -646,8 +671,11 @@
       <c r="C10" s="3">
         <v>0.1323</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -657,8 +685,11 @@
       <c r="C11" s="3">
         <v>0.1323</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -668,8 +699,11 @@
       <c r="C12" s="3">
         <v>0.16170000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -679,8 +713,11 @@
       <c r="C13" s="3">
         <v>0.18151</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -690,8 +727,11 @@
       <c r="C14" s="3">
         <v>0.18276000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -701,8 +741,11 @@
       <c r="C15" s="3">
         <v>0.20077999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -712,8 +755,11 @@
       <c r="C16" s="3">
         <v>0.21182999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -723,8 +769,11 @@
       <c r="C17" s="3">
         <v>0.23580999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -734,8 +783,11 @@
       <c r="C18" s="3">
         <v>0.24986</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -745,8 +797,11 @@
       <c r="C19" s="3">
         <v>0.28239999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -756,8 +811,11 @@
       <c r="C20" s="3">
         <v>0.32549</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -767,8 +825,11 @@
       <c r="C21" s="3">
         <v>0.42009000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -779,7 +840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -790,7 +851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -801,7 +862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -812,7 +873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -823,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -834,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -845,7 +906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -856,7 +917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -867,7 +928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -878,7 +939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1017,7 +1078,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1086,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1039,8 +1100,11 @@
       <c r="D50">
         <v>4.2750000000000003E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1054,8 +1118,11 @@
       <c r="D51">
         <v>4.6780000000000002E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1069,8 +1136,11 @@
       <c r="D52" s="4">
         <v>5.8599999999999999E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1084,8 +1154,11 @@
       <c r="D53" s="4">
         <v>8.2210000000000005E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1099,8 +1172,11 @@
       <c r="D54" s="4">
         <v>8.8400000000000006E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1114,8 +1190,11 @@
       <c r="D55" s="4">
         <v>8.8749999999999996E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1129,8 +1208,11 @@
       <c r="D56" s="5">
         <v>9.461E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1144,16 +1226,22 @@
       <c r="D57" s="4">
         <v>9.5130000000000006E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
       <c r="B58">
         <v>2021</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1167,8 +1255,11 @@
       <c r="D59" s="4">
         <v>0.16853000000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1182,8 +1273,11 @@
       <c r="D60" s="4">
         <v>0.15697</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1197,8 +1291,11 @@
       <c r="D61" s="4">
         <v>0.18657000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1307,7 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -1222,7 +1319,7 @@
       </c>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -1504,13 +1601,6 @@
       <c r="B92">
         <v>2015</v>
       </c>
-      <c r="C92">
-        <f>0.1392+0.06137</f>
-        <v>0.20057</v>
-      </c>
-      <c r="E92" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
@@ -1519,13 +1609,6 @@
       <c r="B93">
         <v>2016</v>
       </c>
-      <c r="C93">
-        <f>0.14578+0.06137</f>
-        <v>0.20715</v>
-      </c>
-      <c r="E93" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -1534,13 +1617,6 @@
       <c r="B94">
         <v>2017</v>
       </c>
-      <c r="C94">
-        <f>0.14872+0.07395</f>
-        <v>0.22266999999999998</v>
-      </c>
-      <c r="E94" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
@@ -1549,13 +1625,6 @@
       <c r="B95">
         <v>2018</v>
       </c>
-      <c r="C95">
-        <f>0.150075+0.08183</f>
-        <v>0.23190499999999997</v>
-      </c>
-      <c r="E95" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -1568,7 +1637,7 @@
         <v>0.16825999999999999</v>
       </c>
       <c r="E96" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -1582,7 +1651,7 @@
         <v>0.17352000000000001</v>
       </c>
       <c r="E97" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -1596,7 +1665,7 @@
         <v>0.17649999999999999</v>
       </c>
       <c r="E98" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -1610,7 +1679,7 @@
         <v>0.19488</v>
       </c>
       <c r="E99" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -1624,7 +1693,7 @@
         <v>0.18856999999999999</v>
       </c>
       <c r="E100" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -1638,7 +1707,7 @@
         <v>0.20041999999999999</v>
       </c>
       <c r="E101" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1648,6 +1717,12 @@
       <c r="B102" s="2">
         <v>2005</v>
       </c>
+      <c r="C102" s="7">
+        <v>7.9799999999999996E-2</v>
+      </c>
+      <c r="E102" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -1656,6 +1731,12 @@
       <c r="B103">
         <v>2006</v>
       </c>
+      <c r="C103" s="7">
+        <v>7.9799999999999996E-2</v>
+      </c>
+      <c r="E103" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
@@ -1664,6 +1745,12 @@
       <c r="B104">
         <v>2007</v>
       </c>
+      <c r="C104" s="7">
+        <v>7.9799999999999996E-2</v>
+      </c>
+      <c r="E104" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
@@ -1672,6 +1759,13 @@
       <c r="B105">
         <v>2008</v>
       </c>
+      <c r="C105" s="7">
+        <f>0.0861+0.001</f>
+        <v>8.7099999999999997E-2</v>
+      </c>
+      <c r="E105" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
@@ -1680,6 +1774,13 @@
       <c r="B106">
         <v>2009</v>
       </c>
+      <c r="C106" s="7">
+        <f>0.0886+0.002</f>
+        <v>9.06E-2</v>
+      </c>
+      <c r="E106" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
@@ -1688,6 +1789,13 @@
       <c r="B107">
         <v>2010</v>
       </c>
+      <c r="C107" s="7">
+        <f>0.0946+0.002</f>
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="E107" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -1696,6 +1804,13 @@
       <c r="B108">
         <v>2011</v>
       </c>
+      <c r="C108" s="7">
+        <f>0.0967+0.0009</f>
+        <v>9.7599999999999992E-2</v>
+      </c>
+      <c r="E108" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
@@ -1704,6 +1819,13 @@
       <c r="B109">
         <v>2012</v>
       </c>
+      <c r="C109" s="7">
+        <f>0.0938+0.0009</f>
+        <v>9.4699999999999993E-2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
@@ -1712,6 +1834,13 @@
       <c r="B110">
         <v>2013</v>
       </c>
+      <c r="C110" s="7">
+        <f>0.0911+0.0013</f>
+        <v>9.2399999999999996E-2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -1720,6 +1849,13 @@
       <c r="B111">
         <v>2014</v>
       </c>
+      <c r="C111" s="7">
+        <f>0.0955+0.0013</f>
+        <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="E111" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -1728,6 +1864,13 @@
       <c r="B112">
         <v>2015</v>
       </c>
+      <c r="C112" s="7">
+        <f>0.0998+0.0015</f>
+        <v>0.1013</v>
+      </c>
+      <c r="E112" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
@@ -1736,6 +1879,12 @@
       <c r="B113">
         <v>2016</v>
       </c>
+      <c r="C113">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="E113" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
@@ -1745,11 +1894,10 @@
         <v>2017</v>
       </c>
       <c r="C114">
-        <f>0.0016+0.1128</f>
-        <v>0.1144</v>
+        <v>0.1128</v>
       </c>
       <c r="E114" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -1760,11 +1908,10 @@
         <v>2018</v>
       </c>
       <c r="C115">
-        <f>0.1032+0.0016</f>
-        <v>0.1048</v>
+        <v>0.1032</v>
       </c>
       <c r="E115" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -1778,7 +1925,7 @@
         <v>0.1032</v>
       </c>
       <c r="E116" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -1789,10 +1936,10 @@
         <v>2020</v>
       </c>
       <c r="C117">
-        <v>0.1032</v>
+        <v>0.1071</v>
       </c>
       <c r="E117" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -1803,10 +1950,10 @@
         <v>2021</v>
       </c>
       <c r="C118">
-        <v>0.1032</v>
+        <v>0.113</v>
       </c>
       <c r="E118" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -1816,6 +1963,12 @@
       <c r="B119">
         <v>2022</v>
       </c>
+      <c r="C119">
+        <v>0.1153</v>
+      </c>
+      <c r="E119" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
@@ -1825,7 +1978,7 @@
         <v>2023</v>
       </c>
       <c r="C120">
-        <v>0.11700000000000001</v>
+        <v>0.11940000000000001</v>
       </c>
       <c r="E120" t="s">
         <v>19</v>
@@ -1842,7 +1995,7 @@
         <v>0.1227</v>
       </c>
       <c r="E121" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>